<commit_message>
After splitting the test train mehod into multiple smaller modules
</commit_message>
<xml_diff>
--- a/EnsembleClassificationTSLA_data_with_prediction.xlsx
+++ b/EnsembleClassificationTSLA_data_with_prediction.xlsx
@@ -643,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -726,10 +726,10 @@
         <v>0</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3">
-        <v>-0.01411042944785268</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -815,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="AD4">
-        <v>-0</v>
+        <v>-0.009458618543870534</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -1070,7 +1070,7 @@
         <v>1</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7">
         <v>0</v>

</xml_diff>